<commit_message>
all: dart fix --dry-run && dart fix --apply
</commit_message>
<xml_diff>
--- a/vergleich.xlsx
+++ b/vergleich.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainf\Desktop\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CB63D2-4055-4887-8BAA-3091DF54E94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56F9119-B2EE-4FED-9AE6-49DC54476F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2625" windowWidth="29040" windowHeight="15720" xr2:uid="{B3930EE7-0CE9-47CB-A31A-101C23E95179}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>95.3%</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Einzigartige Issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Qualitätsmerkmale (Nach flutter fix)</t>
   </si>
 </sst>
 </file>
@@ -563,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A430E050-48F8-40BE-BC32-1DC2CD25A61B}">
   <dimension ref="B2:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -930,7 +936,116 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="10" t="str">
+        <f>E3</f>
+        <v>86.2%</v>
+      </c>
+      <c r="D30" s="10">
+        <v>0</v>
+      </c>
+      <c r="E30" s="10">
+        <v>0</v>
+      </c>
+      <c r="F30" s="10">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="10" t="str">
+        <f t="shared" ref="C31:C33" si="3">E4</f>
+        <v>95.3%</v>
+      </c>
+      <c r="D31" s="10">
+        <v>3</v>
+      </c>
+      <c r="E31" s="10">
+        <v>3</v>
+      </c>
+      <c r="F31" s="10">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>82.9%</v>
+      </c>
+      <c r="D32" s="10">
+        <v>1</v>
+      </c>
+      <c r="E32" s="10">
+        <v>1</v>
+      </c>
+      <c r="F32" s="10">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>85.8%</v>
+      </c>
+      <c r="D33" s="10">
+        <v>5</v>
+      </c>
+      <c r="E33" s="10">
+        <v>4</v>
+      </c>
+      <c r="F33" s="10">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H34" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
python: added script to evaluate flutter analyze output
</commit_message>
<xml_diff>
--- a/vergleich.xlsx
+++ b/vergleich.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainf\Desktop\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56F9119-B2EE-4FED-9AE6-49DC54476F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30E9433-7A9F-4268-9FAA-39CB943A7D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2625" windowWidth="29040" windowHeight="15720" xr2:uid="{B3930EE7-0CE9-47CB-A31A-101C23E95179}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>95.3%</t>
   </si>
@@ -126,6 +126,21 @@
   </si>
   <si>
     <t>Qualitätsmerkmale (Nach flutter fix)</t>
+  </si>
+  <si>
+    <t>inference_failure_on_instance_creation</t>
+  </si>
+  <si>
+    <t>unused_local_variable</t>
+  </si>
+  <si>
+    <t>invalid_use_of_visible_for_testing_member</t>
+  </si>
+  <si>
+    <t>invalid_use_of_protected_member</t>
+  </si>
+  <si>
+    <t>library_private_types_in_public_api (info)</t>
   </si>
 </sst>
 </file>
@@ -203,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -232,6 +247,13 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -567,19 +589,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A430E050-48F8-40BE-BC32-1DC2CD25A61B}">
-  <dimension ref="B2:H34"/>
+  <dimension ref="B2:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="37.90625" customWidth="1"/>
-    <col min="5" max="5" width="30.1796875" customWidth="1"/>
-    <col min="6" max="6" width="28.08984375" customWidth="1"/>
+    <col min="5" max="5" width="26.90625" customWidth="1"/>
+    <col min="6" max="6" width="34.6328125" customWidth="1"/>
     <col min="7" max="7" width="46.26953125" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" customWidth="1"/>
     <col min="9" max="9" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -853,23 +875,23 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="10" t="str">
+      <c r="C22" s="13" t="str">
         <f>E3</f>
         <v>86.2%</v>
       </c>
-      <c r="D22" s="10">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
+      <c r="D22" s="13">
+        <v>0</v>
+      </c>
+      <c r="E22" s="14">
+        <v>0</v>
+      </c>
+      <c r="F22" s="14">
+        <v>0</v>
+      </c>
+      <c r="G22" s="14">
         <v>0</v>
       </c>
     </row>
@@ -986,20 +1008,20 @@
       <c r="B31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="10" t="str">
+      <c r="C31" s="13" t="str">
         <f t="shared" ref="C31:C33" si="3">E4</f>
         <v>95.3%</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="13">
         <v>3</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="13">
         <v>3</v>
       </c>
-      <c r="F31" s="10">
-        <v>0</v>
-      </c>
-      <c r="G31">
+      <c r="F31" s="13">
+        <v>0</v>
+      </c>
+      <c r="G31" s="14">
         <v>2</v>
       </c>
     </row>
@@ -1007,20 +1029,20 @@
       <c r="B32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="10" t="str">
+      <c r="C32" s="13" t="str">
         <f t="shared" si="3"/>
         <v>82.9%</v>
       </c>
-      <c r="D32" s="10">
-        <v>1</v>
-      </c>
-      <c r="E32" s="10">
-        <v>1</v>
-      </c>
-      <c r="F32" s="10">
-        <v>0</v>
-      </c>
-      <c r="G32">
+      <c r="D32" s="13">
+        <v>1</v>
+      </c>
+      <c r="E32" s="13">
+        <v>1</v>
+      </c>
+      <c r="F32" s="13">
+        <v>0</v>
+      </c>
+      <c r="G32" s="14">
         <v>1</v>
       </c>
     </row>
@@ -1028,25 +1050,102 @@
       <c r="B33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="10" t="str">
+      <c r="C33" s="13" t="str">
         <f t="shared" si="3"/>
         <v>85.8%</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="13">
         <v>5</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="13">
         <v>4</v>
       </c>
-      <c r="F33" s="10">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <v>3</v>
+      <c r="F33" s="13">
+        <v>1</v>
+      </c>
+      <c r="G33" s="14">
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D35" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="12">
+        <v>2</v>
+      </c>
+      <c r="E36" s="12">
+        <v>1</v>
+      </c>
+      <c r="F36" s="12">
+        <v>0</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="12">
+        <v>0</v>
+      </c>
+      <c r="E37" s="12">
+        <v>1</v>
+      </c>
+      <c r="F37" s="12">
+        <v>0</v>
+      </c>
+      <c r="G37" s="12">
+        <v>0</v>
+      </c>
+      <c r="H37" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="12">
+        <v>2</v>
+      </c>
+      <c r="E38" s="12">
+        <v>0</v>
+      </c>
+      <c r="F38" s="12">
+        <v>1</v>
+      </c>
+      <c r="G38" s="12">
+        <v>1</v>
+      </c>
+      <c r="H38" s="12">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>